<commit_message>
plantilla actualizada - 1 sprint creditos
</commit_message>
<xml_diff>
--- a/GestionGanadera/recursos/archivos/Plantilla.xlsx
+++ b/GestionGanadera/recursos/archivos/Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\velez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juandavidpaz/git/GestionGanadera1/GestionGanadera/recursos/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A73DE968-C343-42D7-B4D6-733F8021E10E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7B9093-E738-7244-BD77-8968342B012E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{836A19F6-0B98-4636-B64A-92FC2E67E0FA}"/>
+    <workbookView xWindow="3320" yWindow="3280" windowWidth="23260" windowHeight="12720" xr2:uid="{836A19F6-0B98-4636-B64A-92FC2E67E0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,6 +136,7 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,18 +454,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E514D4F6-3A17-4DDD-AC91-A980D66567BF}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Se actualiza la plantilla.
</commit_message>
<xml_diff>
--- a/GestionGanadera/recursos/archivos/Plantilla.xlsx
+++ b/GestionGanadera/recursos/archivos/Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juandavidpaz/git/GestionGanadera1/GestionGanadera/recursos/archivos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\velez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7B9093-E738-7244-BD77-8968342B012E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D71185-7AA5-471E-8E79-58194484AF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="3280" windowWidth="23260" windowHeight="12720" xr2:uid="{836A19F6-0B98-4636-B64A-92FC2E67E0FA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{836A19F6-0B98-4636-B64A-92FC2E67E0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -126,16 +126,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -455,41 +451,42 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="11.5546875" style="3"/>
+    <col min="4" max="4" width="20.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Plantilla e importada definitiva.
</commit_message>
<xml_diff>
--- a/GestionGanadera/recursos/archivos/Plantilla.xlsx
+++ b/GestionGanadera/recursos/archivos/Plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\velez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D71185-7AA5-471E-8E79-58194484AF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCE5C23-834E-43D8-8D34-8EA0E4C96F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{836A19F6-0B98-4636-B64A-92FC2E67E0FA}"/>
+    <workbookView xWindow="2124" yWindow="2136" windowWidth="15336" windowHeight="6720" xr2:uid="{836A19F6-0B98-4636-B64A-92FC2E67E0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +88,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,13 +132,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +458,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +468,7 @@
     <col min="5" max="5" width="8.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -491,6 +498,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>